<commit_message>
TM LED 追記 #41
</commit_message>
<xml_diff>
--- a/資料/設計書/モグラ叩き_TM.xlsx
+++ b/資料/設計書/モグラ叩き_TM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuminori.hakoishi\Desktop\hakoishi\Technical_training\PIC_Micro_Training\C\comp.train.whack-a-mole\資料\設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE167088-EF92-4F6C-8FB0-C3E025374E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A59A33B-41CA-4E84-902C-B1298A348C31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8971E865-DCB4-47C6-BEAD-416AA6065C37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>トレーサビリティマトリクス</t>
     <phoneticPr fontId="2"/>
@@ -394,6 +394,21 @@
   </si>
   <si>
     <t>PWMInterrupt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LED更新</t>
+    <rPh sb="3" eb="5">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>UpdateLED</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -459,7 +474,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -567,13 +582,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -637,6 +663,84 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -658,80 +762,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1047,13 +1091,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0F3352-2B66-409D-8299-E6EAD555EB44}">
-  <dimension ref="A1:AH36"/>
+  <dimension ref="A1:AJ38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="112" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="AE39" sqref="AE39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1065,261 +1109,275 @@
     <col min="5" max="5" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="29" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="30"/>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="31"/>
-    </row>
-    <row r="4" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="40"/>
+    </row>
+    <row r="4" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="21"/>
-      <c r="AD4" s="37" t="s">
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="46"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="46"/>
+      <c r="AB4" s="46"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="AE4" s="42"/>
-      <c r="AF4" s="42"/>
-      <c r="AG4" s="43"/>
-      <c r="AH4" s="47" t="s">
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48" t="s">
+      <c r="E5" s="21"/>
+      <c r="F5" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="34" t="s">
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="41" t="s">
         <v>36</v>
       </c>
       <c r="M5" s="18"/>
-      <c r="N5" s="34" t="s">
+      <c r="N5" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="34" t="s">
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="41" t="s">
         <v>41</v>
       </c>
       <c r="S5" s="18"/>
-      <c r="T5" s="34" t="s">
+      <c r="T5" s="41" t="s">
         <v>43</v>
       </c>
       <c r="U5" s="19"/>
-      <c r="V5" s="34" t="s">
+      <c r="V5" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="26"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="34" t="s">
+      <c r="W5" s="52"/>
+      <c r="X5" s="53"/>
+      <c r="Y5" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="22"/>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="39" t="s">
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE5" s="57"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="AF5" s="40" t="s">
+      <c r="AH5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="47"/>
-    </row>
-    <row r="6" spans="1:34" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="21"/>
+    </row>
+    <row r="6" spans="1:36" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="32" t="s">
+      <c r="E6" s="21"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="51" t="s">
+      <c r="H6" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="L6" s="35"/>
-      <c r="M6" s="32" t="s">
+      <c r="L6" s="42"/>
+      <c r="M6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="32" t="s">
+      <c r="N6" s="42"/>
+      <c r="O6" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="32" t="s">
+      <c r="P6" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="32" t="s">
+      <c r="R6" s="42"/>
+      <c r="S6" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="T6" s="35"/>
-      <c r="U6" s="32" t="s">
+      <c r="T6" s="42"/>
+      <c r="U6" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="V6" s="35"/>
-      <c r="W6" s="32" t="s">
+      <c r="V6" s="42"/>
+      <c r="W6" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="X6" s="32" t="s">
+      <c r="X6" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="32" t="s">
+      <c r="Y6" s="42"/>
+      <c r="Z6" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AA6" s="32" t="s">
+      <c r="AA6" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="AB6" s="32" t="s">
+      <c r="AB6" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="AC6" s="32" t="s">
+      <c r="AC6" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="39"/>
-      <c r="AF6" s="41"/>
-      <c r="AG6" s="28" t="s">
+      <c r="AD6" s="54"/>
+      <c r="AE6" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF6" s="45"/>
+      <c r="AG6" s="32"/>
+      <c r="AH6" s="34"/>
+      <c r="AI6" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="AH6" s="47"/>
-    </row>
-    <row r="7" spans="1:34" s="8" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AJ6" s="21"/>
+    </row>
+    <row r="7" spans="1:36" s="8" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="33"/>
-      <c r="X7" s="33"/>
-      <c r="Y7" s="36"/>
-      <c r="Z7" s="33"/>
-      <c r="AA7" s="33"/>
-      <c r="AB7" s="33"/>
-      <c r="AC7" s="33"/>
-      <c r="AD7" s="38"/>
-      <c r="AE7" s="39"/>
-      <c r="AF7" s="41"/>
-      <c r="AG7" s="28"/>
-      <c r="AH7" s="47"/>
-    </row>
-    <row r="8" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E7" s="21"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="43"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="55"/>
+      <c r="AE7" s="58"/>
+      <c r="AF7" s="45"/>
+      <c r="AG7" s="32"/>
+      <c r="AH7" s="34"/>
+      <c r="AI7" s="37"/>
+      <c r="AJ7" s="21"/>
+    </row>
+    <row r="8" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="17">
         <f>ROW(A8) - 7</f>
         <v>1</v>
@@ -1358,11 +1416,13 @@
       <c r="AE8" s="12"/>
       <c r="AF8" s="12"/>
       <c r="AG8" s="12"/>
-      <c r="AH8" s="10"/>
-    </row>
-    <row r="9" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AH8" s="12"/>
+      <c r="AI8" s="12"/>
+      <c r="AJ8" s="10"/>
+    </row>
+    <row r="9" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="17">
-        <f t="shared" ref="A9:A36" si="0">ROW(A9) - 7</f>
+        <f t="shared" ref="A9:A38" si="0">ROW(A9) - 7</f>
         <v>2</v>
       </c>
       <c r="B9" s="14"/>
@@ -1397,13 +1457,15 @@
       <c r="AA9" s="13"/>
       <c r="AB9" s="13"/>
       <c r="AC9" s="13"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
       <c r="AF9" s="10"/>
       <c r="AG9" s="10"/>
       <c r="AH9" s="10"/>
-    </row>
-    <row r="10" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI9" s="10"/>
+      <c r="AJ9" s="10"/>
+    </row>
+    <row r="10" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1440,13 +1502,15 @@
       <c r="AA10" s="13"/>
       <c r="AB10" s="13"/>
       <c r="AC10" s="13"/>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="10"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="10"/>
-    </row>
-    <row r="11" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="10"/>
+    </row>
+    <row r="11" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1481,13 +1545,15 @@
       <c r="AA11" s="13"/>
       <c r="AB11" s="13"/>
       <c r="AC11" s="13"/>
-      <c r="AD11" s="10"/>
-      <c r="AE11" s="10"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
       <c r="AF11" s="10"/>
       <c r="AG11" s="10"/>
       <c r="AH11" s="10"/>
-    </row>
-    <row r="12" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI11" s="10"/>
+      <c r="AJ11" s="10"/>
+    </row>
+    <row r="12" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1526,13 +1592,15 @@
       <c r="AA12" s="13"/>
       <c r="AB12" s="13"/>
       <c r="AC12" s="13"/>
-      <c r="AD12" s="10"/>
-      <c r="AE12" s="10"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
       <c r="AF12" s="10"/>
       <c r="AG12" s="10"/>
       <c r="AH12" s="10"/>
-    </row>
-    <row r="13" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI12" s="10"/>
+      <c r="AJ12" s="10"/>
+    </row>
+    <row r="13" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="17">
         <v>6</v>
       </c>
@@ -1568,13 +1636,15 @@
       <c r="AA13" s="13"/>
       <c r="AB13" s="13"/>
       <c r="AC13" s="13"/>
-      <c r="AD13" s="10"/>
-      <c r="AE13" s="10"/>
+      <c r="AD13" s="13"/>
+      <c r="AE13" s="13"/>
       <c r="AF13" s="10"/>
       <c r="AG13" s="10"/>
       <c r="AH13" s="10"/>
-    </row>
-    <row r="14" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="10"/>
+    </row>
+    <row r="14" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="17">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1611,13 +1681,15 @@
       <c r="AA14" s="13"/>
       <c r="AB14" s="13"/>
       <c r="AC14" s="13"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
+      <c r="AD14" s="13"/>
+      <c r="AE14" s="13"/>
       <c r="AF14" s="10"/>
       <c r="AG14" s="10"/>
       <c r="AH14" s="10"/>
-    </row>
-    <row r="15" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI14" s="10"/>
+      <c r="AJ14" s="10"/>
+    </row>
+    <row r="15" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1654,13 +1726,15 @@
       <c r="AA15" s="13"/>
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="10"/>
+      <c r="AD15" s="13"/>
+      <c r="AE15" s="13"/>
       <c r="AF15" s="10"/>
       <c r="AG15" s="10"/>
       <c r="AH15" s="10"/>
-    </row>
-    <row r="16" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI15" s="10"/>
+      <c r="AJ15" s="10"/>
+    </row>
+    <row r="16" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1695,13 +1769,15 @@
       <c r="AA16" s="13"/>
       <c r="AB16" s="13"/>
       <c r="AC16" s="13"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="10"/>
+      <c r="AD16" s="13"/>
+      <c r="AE16" s="13"/>
       <c r="AF16" s="10"/>
       <c r="AG16" s="10"/>
       <c r="AH16" s="10"/>
-    </row>
-    <row r="17" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI16" s="10"/>
+      <c r="AJ16" s="10"/>
+    </row>
+    <row r="17" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1736,15 +1812,17 @@
       <c r="AA17" s="13"/>
       <c r="AB17" s="13"/>
       <c r="AC17" s="13"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="13"/>
       <c r="AF17" s="10"/>
-      <c r="AG17" s="10" t="s">
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AH17" s="10"/>
-    </row>
-    <row r="18" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AJ17" s="10"/>
+    </row>
+    <row r="18" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1781,13 +1859,15 @@
       <c r="AA18" s="13"/>
       <c r="AB18" s="13"/>
       <c r="AC18" s="13"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
+      <c r="AD18" s="13"/>
+      <c r="AE18" s="13"/>
       <c r="AF18" s="10"/>
       <c r="AG18" s="10"/>
       <c r="AH18" s="10"/>
-    </row>
-    <row r="19" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI18" s="10"/>
+      <c r="AJ18" s="10"/>
+    </row>
+    <row r="19" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1822,13 +1902,15 @@
       <c r="AA19" s="13"/>
       <c r="AB19" s="13"/>
       <c r="AC19" s="13"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="10"/>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
       <c r="AF19" s="10"/>
       <c r="AG19" s="10"/>
       <c r="AH19" s="10"/>
-    </row>
-    <row r="20" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI19" s="10"/>
+      <c r="AJ19" s="10"/>
+    </row>
+    <row r="20" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1865,13 +1947,15 @@
       <c r="AA20" s="13"/>
       <c r="AB20" s="13"/>
       <c r="AC20" s="13"/>
-      <c r="AD20" s="10"/>
-      <c r="AE20" s="10"/>
+      <c r="AD20" s="13"/>
+      <c r="AE20" s="13"/>
       <c r="AF20" s="10"/>
       <c r="AG20" s="10"/>
       <c r="AH20" s="10"/>
-    </row>
-    <row r="21" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI20" s="10"/>
+      <c r="AJ20" s="10"/>
+    </row>
+    <row r="21" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="17">
         <f>ROW(A21) - 7</f>
         <v>14</v>
@@ -1906,13 +1990,15 @@
       <c r="AA21" s="13"/>
       <c r="AB21" s="13"/>
       <c r="AC21" s="13"/>
-      <c r="AD21" s="10"/>
-      <c r="AE21" s="10"/>
+      <c r="AD21" s="13"/>
+      <c r="AE21" s="13"/>
       <c r="AF21" s="10"/>
       <c r="AG21" s="10"/>
       <c r="AH21" s="10"/>
-    </row>
-    <row r="22" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI21" s="10"/>
+      <c r="AJ21" s="10"/>
+    </row>
+    <row r="22" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="17">
         <f>ROW(A22) - 7</f>
         <v>15</v>
@@ -1949,13 +2035,15 @@
       <c r="AA22" s="13"/>
       <c r="AB22" s="13"/>
       <c r="AC22" s="13"/>
-      <c r="AD22" s="10"/>
-      <c r="AE22" s="10"/>
+      <c r="AD22" s="13"/>
+      <c r="AE22" s="13"/>
       <c r="AF22" s="10"/>
       <c r="AG22" s="10"/>
       <c r="AH22" s="10"/>
-    </row>
-    <row r="23" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI22" s="10"/>
+      <c r="AJ22" s="10"/>
+    </row>
+    <row r="23" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="17">
         <f>ROW(A23) - 7</f>
         <v>16</v>
@@ -1992,13 +2080,15 @@
       <c r="AA23" s="13"/>
       <c r="AB23" s="13"/>
       <c r="AC23" s="13"/>
-      <c r="AD23" s="10"/>
-      <c r="AE23" s="10"/>
+      <c r="AD23" s="13"/>
+      <c r="AE23" s="13"/>
       <c r="AF23" s="10"/>
       <c r="AG23" s="10"/>
       <c r="AH23" s="10"/>
-    </row>
-    <row r="24" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI23" s="10"/>
+      <c r="AJ23" s="10"/>
+    </row>
+    <row r="24" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2035,13 +2125,15 @@
       <c r="AA24" s="13"/>
       <c r="AB24" s="13"/>
       <c r="AC24" s="13"/>
-      <c r="AD24" s="10"/>
-      <c r="AE24" s="10"/>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="13"/>
       <c r="AF24" s="10"/>
       <c r="AG24" s="10"/>
       <c r="AH24" s="10"/>
-    </row>
-    <row r="25" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI24" s="10"/>
+      <c r="AJ24" s="10"/>
+    </row>
+    <row r="25" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="17">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2078,13 +2170,15 @@
       <c r="AA25" s="13"/>
       <c r="AB25" s="13"/>
       <c r="AC25" s="13"/>
-      <c r="AD25" s="10"/>
-      <c r="AE25" s="10"/>
+      <c r="AD25" s="13"/>
+      <c r="AE25" s="13"/>
       <c r="AF25" s="10"/>
       <c r="AG25" s="10"/>
       <c r="AH25" s="10"/>
-    </row>
-    <row r="26" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI25" s="10"/>
+      <c r="AJ25" s="10"/>
+    </row>
+    <row r="26" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="17">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2119,13 +2213,15 @@
       <c r="AA26" s="13"/>
       <c r="AB26" s="13"/>
       <c r="AC26" s="13"/>
-      <c r="AD26" s="10"/>
-      <c r="AE26" s="10"/>
+      <c r="AD26" s="13"/>
+      <c r="AE26" s="13"/>
       <c r="AF26" s="10"/>
       <c r="AG26" s="10"/>
       <c r="AH26" s="10"/>
-    </row>
-    <row r="27" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI26" s="10"/>
+      <c r="AJ26" s="10"/>
+    </row>
+    <row r="27" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="17">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2160,15 +2256,17 @@
       <c r="AA27" s="13"/>
       <c r="AB27" s="13"/>
       <c r="AC27" s="13"/>
-      <c r="AD27" s="10"/>
-      <c r="AE27" s="10" t="s">
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="13"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AF27" s="10"/>
-      <c r="AG27" s="10"/>
       <c r="AH27" s="10"/>
-    </row>
-    <row r="28" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI27" s="10"/>
+      <c r="AJ27" s="10"/>
+    </row>
+    <row r="28" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="17">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2203,13 +2301,15 @@
       <c r="AA28" s="13"/>
       <c r="AB28" s="13"/>
       <c r="AC28" s="13"/>
-      <c r="AD28" s="10"/>
-      <c r="AE28" s="10"/>
+      <c r="AD28" s="13"/>
+      <c r="AE28" s="13"/>
       <c r="AF28" s="10"/>
       <c r="AG28" s="10"/>
       <c r="AH28" s="10"/>
-    </row>
-    <row r="29" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI28" s="10"/>
+      <c r="AJ28" s="10"/>
+    </row>
+    <row r="29" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="17">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2244,13 +2344,15 @@
       <c r="AA29" s="13"/>
       <c r="AB29" s="13"/>
       <c r="AC29" s="13"/>
-      <c r="AD29" s="10"/>
-      <c r="AE29" s="10"/>
+      <c r="AD29" s="13"/>
+      <c r="AE29" s="13"/>
       <c r="AF29" s="10"/>
       <c r="AG29" s="10"/>
       <c r="AH29" s="10"/>
-    </row>
-    <row r="30" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI29" s="10"/>
+      <c r="AJ29" s="10"/>
+    </row>
+    <row r="30" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="17">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2287,13 +2389,15 @@
       <c r="AA30" s="13"/>
       <c r="AB30" s="13"/>
       <c r="AC30" s="13"/>
-      <c r="AD30" s="10"/>
-      <c r="AE30" s="10"/>
+      <c r="AD30" s="13"/>
+      <c r="AE30" s="13"/>
       <c r="AF30" s="10"/>
       <c r="AG30" s="10"/>
       <c r="AH30" s="10"/>
-    </row>
-    <row r="31" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI30" s="10"/>
+      <c r="AJ30" s="10"/>
+    </row>
+    <row r="31" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="17">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2330,13 +2434,15 @@
       <c r="AA31" s="13"/>
       <c r="AB31" s="13"/>
       <c r="AC31" s="13"/>
-      <c r="AD31" s="10"/>
-      <c r="AE31" s="10"/>
+      <c r="AD31" s="13"/>
+      <c r="AE31" s="13"/>
       <c r="AF31" s="10"/>
       <c r="AG31" s="10"/>
       <c r="AH31" s="10"/>
-    </row>
-    <row r="32" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI31" s="10"/>
+      <c r="AJ31" s="10"/>
+    </row>
+    <row r="32" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="17">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2371,13 +2477,15 @@
       <c r="AA32" s="13"/>
       <c r="AB32" s="13"/>
       <c r="AC32" s="13"/>
-      <c r="AD32" s="10"/>
-      <c r="AE32" s="10"/>
+      <c r="AD32" s="13"/>
+      <c r="AE32" s="13"/>
       <c r="AF32" s="10"/>
       <c r="AG32" s="10"/>
       <c r="AH32" s="10"/>
-    </row>
-    <row r="33" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AI32" s="10"/>
+      <c r="AJ32" s="10"/>
+    </row>
+    <row r="33" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="17">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2414,15 +2522,17 @@
       <c r="AA33" s="13"/>
       <c r="AB33" s="13"/>
       <c r="AC33" s="13"/>
-      <c r="AD33" s="10"/>
-      <c r="AE33" s="10"/>
+      <c r="AD33" s="13"/>
+      <c r="AE33" s="13"/>
       <c r="AF33" s="10"/>
       <c r="AG33" s="10"/>
-      <c r="AH33" s="10" t="s">
+      <c r="AH33" s="10"/>
+      <c r="AI33" s="10"/>
+      <c r="AJ33" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="17">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2459,15 +2569,17 @@
       </c>
       <c r="AB34" s="13"/>
       <c r="AC34" s="13"/>
-      <c r="AD34" s="10"/>
-      <c r="AE34" s="10"/>
+      <c r="AD34" s="13"/>
+      <c r="AE34" s="13"/>
       <c r="AF34" s="10"/>
       <c r="AG34" s="10"/>
-      <c r="AH34" s="10" t="s">
+      <c r="AH34" s="10"/>
+      <c r="AI34" s="10"/>
+      <c r="AJ34" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="17">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2504,20 +2616,22 @@
         <v>29</v>
       </c>
       <c r="AC35" s="13"/>
-      <c r="AD35" s="10"/>
-      <c r="AE35" s="10"/>
+      <c r="AD35" s="13"/>
+      <c r="AE35" s="13"/>
       <c r="AF35" s="10"/>
       <c r="AG35" s="10"/>
-      <c r="AH35" s="10" t="s">
+      <c r="AH35" s="10"/>
+      <c r="AI35" s="10"/>
+      <c r="AJ35" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="17">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B36" s="12"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="12"/>
       <c r="D36" s="10" t="s">
         <v>52</v>
@@ -2549,35 +2663,123 @@
       <c r="AC36" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AD36" s="10"/>
-      <c r="AE36" s="10"/>
+      <c r="AD36" s="13"/>
+      <c r="AE36" s="13"/>
       <c r="AF36" s="10"/>
       <c r="AG36" s="10"/>
-      <c r="AH36" s="10" t="s">
+      <c r="AH36" s="10"/>
+      <c r="AI36" s="10"/>
+      <c r="AJ36" s="10" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="37" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="17">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="15"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="13"/>
+      <c r="Y37" s="13"/>
+      <c r="Z37" s="13"/>
+      <c r="AA37" s="13"/>
+      <c r="AB37" s="13"/>
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="13"/>
+      <c r="AF37" s="13"/>
+      <c r="AG37" s="13"/>
+      <c r="AH37" s="13"/>
+      <c r="AI37" s="13"/>
+      <c r="AJ37" s="13"/>
+    </row>
+    <row r="38" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="17">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="13"/>
+      <c r="X38" s="13"/>
+      <c r="Y38" s="13"/>
+      <c r="Z38" s="13"/>
+      <c r="AA38" s="13"/>
+      <c r="AB38" s="13"/>
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="13"/>
+      <c r="AE38" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF38" s="13"/>
+      <c r="AG38" s="13"/>
+      <c r="AH38" s="13"/>
+      <c r="AI38" s="13"/>
+      <c r="AJ38" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="AH4:AH7"/>
-    <mergeCell ref="AC6:AC7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="P6:P7"/>
+  <mergeCells count="40">
+    <mergeCell ref="AF4:AF7"/>
+    <mergeCell ref="F4:AC4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="AD5:AD7"/>
+    <mergeCell ref="AE6:AE7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="AB6:AB7"/>
     <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AE5:AE7"/>
-    <mergeCell ref="AF5:AF7"/>
-    <mergeCell ref="AE4:AG4"/>
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="X6:X7"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="E3:AH3"/>
+    <mergeCell ref="E3:AJ3"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L5:L7"/>
     <mergeCell ref="M6:M7"/>
@@ -2585,18 +2787,22 @@
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="R5:R7"/>
     <mergeCell ref="S6:S7"/>
+    <mergeCell ref="AJ4:AJ7"/>
+    <mergeCell ref="AC6:AC7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="AG5:AG7"/>
+    <mergeCell ref="AH5:AH7"/>
+    <mergeCell ref="AG4:AI4"/>
+    <mergeCell ref="AI6:AI7"/>
     <mergeCell ref="T5:T7"/>
     <mergeCell ref="U6:U7"/>
     <mergeCell ref="V5:V7"/>
     <mergeCell ref="W6:W7"/>
     <mergeCell ref="Y5:Y7"/>
     <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AD4:AD7"/>
-    <mergeCell ref="F4:AC4"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Z5:AC5"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>